<commit_message>
Cleaned up spelling/capitalization in my original assessment
</commit_message>
<xml_diff>
--- a/reports/Protocol_test_Kendall.xlsx
+++ b/reports/Protocol_test_Kendall.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendall/Documents/Github/MPM-errors/reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bkendall/Documents/github-bitbucket/MPM-errors/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1EF19FEC-55A3-C344-84ED-C476FB8675E6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2096B904-443B-0C41-833C-72ABC04728BE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
+    <workbookView xWindow="760" yWindow="560" windowWidth="32560" windowHeight="19940" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="208">
   <si>
     <t>CompadrinoName</t>
   </si>
@@ -237,9 +237,6 @@
     <t>10.1002/ece3.984</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Chitwood; Lashley; Kilgo; Moorman; Deperno</t>
   </si>
   <si>
@@ -519,30 +516,6 @@
     <t>Typo in DOI</t>
   </si>
   <si>
-    <t>post</t>
-  </si>
-  <si>
-    <t>pre</t>
-  </si>
-  <si>
-    <t>unk</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>offspring</t>
-  </si>
-  <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>1 | 2 | 3 | 4 | 5</t>
   </si>
   <si>
@@ -612,27 +585,9 @@
     <t>3.87 | 6.58 | 7.75 | 7.5 | 3.68 | 6.94</t>
   </si>
   <si>
-    <t>calculate</t>
-  </si>
-  <si>
-    <t>observed</t>
-  </si>
-  <si>
-    <t>cohort</t>
-  </si>
-  <si>
-    <t>unrolled</t>
-  </si>
-  <si>
     <t>1/T</t>
   </si>
   <si>
-    <t>Crouse</t>
-  </si>
-  <si>
-    <t>Caswell 6.103</t>
-  </si>
-  <si>
     <t>GeneralObs</t>
   </si>
   <si>
@@ -688,6 +643,12 @@
   </si>
   <si>
     <t>comadre has multiple years but from just one species; matrices not in paper</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>Sub-adults</t>
   </si>
 </sst>
 </file>
@@ -1051,12 +1012,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC16C70-3AD3-0840-9DA4-3FC542326147}">
   <dimension ref="A1:AK43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane xSplit="3" ySplit="11" topLeftCell="AC12" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="6" ySplit="11" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
-      <selection pane="bottomRight" activeCell="AJ31" sqref="AJ31"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1201,7 +1161,7 @@
         <v>38</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
@@ -1362,42 +1322,39 @@
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" t="s">
         <v>155</v>
-      </c>
-      <c r="D12" t="s">
-        <v>156</v>
       </c>
       <c r="E12">
         <v>2015</v>
       </c>
       <c r="F12" t="s">
-        <v>157</v>
-      </c>
-      <c r="G12" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
       <c r="S12" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U12" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA12" t="b">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>9</v>
       </c>
       <c r="AC12" s="2" t="s">
-        <v>171</v>
+        <v>16</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AI12" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D13" t="s">
         <v>68</v>
@@ -1408,128 +1365,116 @@
       <c r="F13" t="s">
         <v>69</v>
       </c>
-      <c r="G13" t="s">
-        <v>70</v>
-      </c>
       <c r="S13" t="s">
-        <v>165</v>
+        <v>10</v>
       </c>
       <c r="U13" t="s">
-        <v>168</v>
-      </c>
-      <c r="AA13" t="b">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>8</v>
       </c>
       <c r="AC13" s="2" t="s">
-        <v>171</v>
+        <v>16</v>
       </c>
       <c r="AE13" s="2" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AI13" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AK13" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" t="s">
         <v>71</v>
-      </c>
-      <c r="D14" t="s">
-        <v>72</v>
       </c>
       <c r="E14">
         <v>2015</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="S14" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AA14" t="b">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>8</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>171</v>
+        <v>16</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AI14" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" t="s">
         <v>74</v>
-      </c>
-      <c r="D15" t="s">
-        <v>75</v>
       </c>
       <c r="E15">
         <v>2012</v>
       </c>
       <c r="F15" t="s">
-        <v>76</v>
-      </c>
-      <c r="G15" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="S15" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U15" t="s">
-        <v>169</v>
-      </c>
-      <c r="AA15" t="b">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>8</v>
       </c>
       <c r="AC15" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="AI15" t="s">
-        <v>195</v>
+        <v>43</v>
       </c>
       <c r="AK15" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" t="s">
         <v>77</v>
-      </c>
-      <c r="D16" t="s">
-        <v>78</v>
       </c>
       <c r="E16">
         <v>2015</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="S16" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U16" t="s">
-        <v>169</v>
-      </c>
-      <c r="AA16" t="b">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>8</v>
       </c>
       <c r="AC16" s="2">
         <v>2</v>
@@ -1538,36 +1483,36 @@
         <v>3</v>
       </c>
       <c r="AI16" t="s">
-        <v>196</v>
+        <v>28</v>
       </c>
       <c r="AK16" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" t="s">
         <v>80</v>
-      </c>
-      <c r="D17" t="s">
-        <v>81</v>
       </c>
       <c r="E17">
         <v>2011</v>
       </c>
       <c r="F17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" t="s">
         <v>82</v>
       </c>
-      <c r="G17" t="s">
-        <v>83</v>
-      </c>
       <c r="S17" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U17" t="s">
-        <v>167</v>
+        <v>16</v>
       </c>
       <c r="AA17" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="AC17" s="2">
         <v>0</v>
@@ -1576,36 +1521,33 @@
         <v>0</v>
       </c>
       <c r="AI17" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AK17" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
         <v>84</v>
-      </c>
-      <c r="D18" t="s">
-        <v>85</v>
       </c>
       <c r="E18">
         <v>2011</v>
       </c>
       <c r="F18" t="s">
-        <v>86</v>
-      </c>
-      <c r="G18" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="S18" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U18" t="s">
-        <v>169</v>
-      </c>
-      <c r="AA18" t="b">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>8</v>
       </c>
       <c r="AC18" s="2">
         <v>2</v>
@@ -1614,36 +1556,33 @@
         <v>2</v>
       </c>
       <c r="AI18" t="s">
-        <v>196</v>
+        <v>28</v>
       </c>
       <c r="AK18" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E19">
         <v>2014</v>
       </c>
       <c r="F19" t="s">
-        <v>88</v>
-      </c>
-      <c r="G19" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="S19" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U19" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA19" t="b">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>9</v>
       </c>
       <c r="AC19" s="2">
         <v>0</v>
@@ -1652,80 +1591,74 @@
         <v>0</v>
       </c>
       <c r="AI19" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AK19" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" t="s">
         <v>89</v>
-      </c>
-      <c r="D20" t="s">
-        <v>90</v>
       </c>
       <c r="E20">
         <v>2014</v>
       </c>
       <c r="F20" t="s">
-        <v>91</v>
-      </c>
-      <c r="G20" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="K20" t="s">
+        <v>161</v>
+      </c>
+      <c r="L20" t="s">
         <v>162</v>
       </c>
-      <c r="L20" t="s">
-        <v>163</v>
-      </c>
       <c r="S20" t="s">
+        <v>11</v>
+      </c>
+      <c r="U20" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC20" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="U20" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA20" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="2" t="s">
-        <v>173</v>
-      </c>
       <c r="AE20" s="2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="AI20" t="s">
-        <v>195</v>
+        <v>43</v>
       </c>
       <c r="AK20" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" t="s">
         <v>92</v>
-      </c>
-      <c r="D21" t="s">
-        <v>93</v>
       </c>
       <c r="E21">
         <v>2013</v>
       </c>
       <c r="F21" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="S21" t="s">
-        <v>165</v>
+        <v>10</v>
       </c>
       <c r="U21" t="s">
-        <v>168</v>
-      </c>
-      <c r="AA21" t="b">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>8</v>
       </c>
       <c r="AC21" s="2">
         <v>0</v>
@@ -1734,36 +1667,33 @@
         <v>0</v>
       </c>
       <c r="AI21" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AK21" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" t="s">
         <v>95</v>
-      </c>
-      <c r="D22" t="s">
-        <v>96</v>
       </c>
       <c r="E22">
         <v>2014</v>
       </c>
       <c r="F22" t="s">
-        <v>97</v>
-      </c>
-      <c r="G22" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="S22" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U22" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="AA22" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="AC22" s="2">
         <v>0</v>
@@ -1772,714 +1702,669 @@
         <v>0</v>
       </c>
       <c r="AI22" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AK22" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" t="s">
         <v>98</v>
-      </c>
-      <c r="D23" t="s">
-        <v>99</v>
       </c>
       <c r="E23">
         <v>2014</v>
       </c>
       <c r="F23" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="S23" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U23" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA23" t="b">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>9</v>
       </c>
       <c r="AC23" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="AE23" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="AI23" t="s">
-        <v>197</v>
+        <v>27</v>
       </c>
       <c r="AK23" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
         <v>101</v>
-      </c>
-      <c r="D24" t="s">
-        <v>102</v>
       </c>
       <c r="E24">
         <v>2012</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
-      </c>
-      <c r="G24" t="s">
-        <v>70</v>
+        <v>102</v>
+      </c>
+      <c r="M24" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24" t="s">
+        <v>197</v>
       </c>
       <c r="S24" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U24" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA24" t="b">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>9</v>
       </c>
       <c r="AC24" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="AE24" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="AI24" t="s">
-        <v>198</v>
-      </c>
-      <c r="AK24" t="s">
-        <v>212</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E25">
         <v>2012</v>
       </c>
       <c r="F25" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="S25" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U25" t="s">
-        <v>169</v>
-      </c>
-      <c r="AA25" t="b">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>8</v>
       </c>
       <c r="AC25" s="2" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="AE25" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="AI25" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="AK25" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E26">
         <v>2014</v>
       </c>
       <c r="F26" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="S26" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U26" t="s">
-        <v>169</v>
-      </c>
-      <c r="AA26" t="b">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>9</v>
       </c>
       <c r="AC26" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="AE26" s="2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="AI26" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E27">
         <v>2015</v>
       </c>
       <c r="F27" t="s">
-        <v>109</v>
-      </c>
-      <c r="G27" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="S27" t="s">
-        <v>165</v>
+        <v>10</v>
       </c>
       <c r="U27" t="s">
-        <v>168</v>
-      </c>
-      <c r="AA27" t="b">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>8</v>
       </c>
       <c r="AC27" s="2" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="AE27" s="2" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="AI27" t="s">
-        <v>198</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E28">
         <v>2015</v>
       </c>
       <c r="F28" t="s">
-        <v>111</v>
-      </c>
-      <c r="G28" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="S28" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U28" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AA28" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AC28" s="2" t="s">
-        <v>171</v>
+        <v>16</v>
       </c>
       <c r="AE28" s="2" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AI28" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AK28" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E29">
         <v>2015</v>
       </c>
       <c r="F29" t="s">
-        <v>113</v>
-      </c>
-      <c r="G29" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="S29" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U29" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA29" t="b">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>9</v>
       </c>
       <c r="AC29" s="2" t="s">
-        <v>171</v>
+        <v>16</v>
       </c>
       <c r="AE29" s="2" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AI29" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AK29" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" t="s">
         <v>114</v>
-      </c>
-      <c r="D30" t="s">
-        <v>115</v>
       </c>
       <c r="E30">
         <v>2013</v>
       </c>
       <c r="F30" t="s">
-        <v>116</v>
-      </c>
-      <c r="G30" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="S30" t="s">
-        <v>165</v>
+        <v>10</v>
       </c>
       <c r="U30" t="s">
-        <v>168</v>
-      </c>
-      <c r="AA30" t="b">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>8</v>
       </c>
       <c r="AC30" s="2" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="AE30" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="AI30" t="s">
-        <v>198</v>
+        <v>29</v>
       </c>
       <c r="AK30" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" t="s">
         <v>117</v>
-      </c>
-      <c r="D31" t="s">
-        <v>118</v>
       </c>
       <c r="E31">
         <v>2013</v>
       </c>
       <c r="F31" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" t="s">
         <v>119</v>
-      </c>
-      <c r="G31" t="s">
-        <v>120</v>
       </c>
       <c r="AC31" s="2"/>
       <c r="AE31" s="2"/>
       <c r="AK31" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" t="s">
         <v>117</v>
-      </c>
-      <c r="D32" t="s">
-        <v>118</v>
       </c>
       <c r="E32">
         <v>2013</v>
       </c>
       <c r="F32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC32" s="2"/>
       <c r="AE32" s="2"/>
       <c r="AK32" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" t="s">
         <v>122</v>
-      </c>
-      <c r="D33" t="s">
-        <v>123</v>
       </c>
       <c r="E33">
         <v>2012</v>
       </c>
       <c r="F33" t="s">
-        <v>124</v>
-      </c>
-      <c r="G33" t="s">
-        <v>70</v>
+        <v>123</v>
       </c>
       <c r="S33" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="U33" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="AA33" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="AC33" s="2" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="AE33" s="2" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="AI33" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="AK33" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34" t="s">
         <v>125</v>
-      </c>
-      <c r="D34" t="s">
-        <v>126</v>
       </c>
       <c r="E34">
         <v>2013</v>
       </c>
       <c r="F34" t="s">
-        <v>127</v>
-      </c>
-      <c r="G34" t="s">
-        <v>70</v>
+        <v>126</v>
       </c>
       <c r="S34" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U34" t="s">
-        <v>169</v>
-      </c>
-      <c r="AA34" t="b">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>9</v>
       </c>
       <c r="AC34" s="2" t="s">
-        <v>175</v>
+        <v>207</v>
       </c>
       <c r="AE34" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="AI34" t="s">
-        <v>200</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
+        <v>127</v>
+      </c>
+      <c r="D35" t="s">
         <v>128</v>
-      </c>
-      <c r="D35" t="s">
-        <v>129</v>
       </c>
       <c r="E35">
         <v>2013</v>
       </c>
       <c r="F35" t="s">
-        <v>130</v>
-      </c>
-      <c r="G35" t="s">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="AC35" s="2"/>
       <c r="AE35" s="2"/>
     </row>
     <row r="36" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" t="s">
         <v>131</v>
-      </c>
-      <c r="D36" t="s">
-        <v>132</v>
       </c>
       <c r="E36">
         <v>2012</v>
       </c>
       <c r="F36" t="s">
-        <v>133</v>
-      </c>
-      <c r="G36" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="AC36" s="2"/>
       <c r="AE36" s="2"/>
       <c r="AK36" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" t="s">
         <v>134</v>
-      </c>
-      <c r="D37" t="s">
-        <v>135</v>
       </c>
       <c r="E37">
         <v>2013</v>
       </c>
       <c r="F37" t="s">
-        <v>136</v>
-      </c>
-      <c r="G37" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="S37" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U37" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA37" t="b">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>9</v>
       </c>
       <c r="AC37" s="2" t="s">
-        <v>167</v>
+        <v>16</v>
       </c>
       <c r="AE37" s="2" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AI37" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" t="s">
         <v>137</v>
-      </c>
-      <c r="D38" t="s">
-        <v>138</v>
       </c>
       <c r="E38">
         <v>2011</v>
       </c>
       <c r="F38" t="s">
+        <v>138</v>
+      </c>
+      <c r="G38" t="s">
         <v>139</v>
       </c>
-      <c r="G38" t="s">
-        <v>140</v>
-      </c>
       <c r="S38" t="s">
-        <v>165</v>
+        <v>10</v>
       </c>
       <c r="U38" t="s">
-        <v>168</v>
-      </c>
-      <c r="AA38" t="b">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>8</v>
       </c>
       <c r="AC38" s="2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="AE38" s="2">
         <v>7</v>
       </c>
       <c r="AI38" t="s">
-        <v>198</v>
+        <v>29</v>
       </c>
       <c r="AK38" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39" t="s">
         <v>141</v>
-      </c>
-      <c r="D39" t="s">
-        <v>142</v>
       </c>
       <c r="E39">
         <v>2014</v>
       </c>
       <c r="F39" t="s">
-        <v>143</v>
-      </c>
-      <c r="G39" t="s">
-        <v>70</v>
+        <v>142</v>
       </c>
       <c r="S39" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U39" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA39" t="b">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>9</v>
       </c>
       <c r="AC39" s="2" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="AE39" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="AI39" t="s">
-        <v>201</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
+        <v>143</v>
+      </c>
+      <c r="D40" t="s">
         <v>144</v>
-      </c>
-      <c r="D40" t="s">
-        <v>145</v>
       </c>
       <c r="E40">
         <v>2015</v>
       </c>
       <c r="F40" t="s">
-        <v>146</v>
-      </c>
-      <c r="G40" t="s">
-        <v>70</v>
+        <v>145</v>
       </c>
       <c r="S40" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U40" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA40" t="b">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>9</v>
       </c>
       <c r="AC40" s="2" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="AE40" s="2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="AI40" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E41">
         <v>2016</v>
       </c>
       <c r="F41" t="s">
-        <v>148</v>
-      </c>
-      <c r="G41" t="s">
-        <v>70</v>
+        <v>147</v>
       </c>
       <c r="S41" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U41" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="AA41" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="AC41" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="AE41" s="2" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="AI41" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
+        <v>148</v>
+      </c>
+      <c r="D42" t="s">
         <v>149</v>
-      </c>
-      <c r="D42" t="s">
-        <v>150</v>
       </c>
       <c r="E42">
         <v>2013</v>
       </c>
       <c r="F42" t="s">
+        <v>150</v>
+      </c>
+      <c r="G42" t="s">
         <v>151</v>
       </c>
-      <c r="G42" t="s">
-        <v>152</v>
-      </c>
       <c r="S42" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U42" t="s">
-        <v>169</v>
-      </c>
-      <c r="AA42" t="b">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>8</v>
       </c>
       <c r="AC42" s="2" t="s">
-        <v>167</v>
+        <v>16</v>
       </c>
       <c r="AE42" s="2" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AI42" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
     </row>
     <row r="43" spans="3:37" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E43">
         <v>2014</v>
       </c>
       <c r="F43" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S43" t="s">
-        <v>164</v>
+        <v>11</v>
       </c>
       <c r="U43" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA43" t="b">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>8</v>
       </c>
       <c r="AC43" s="2" t="s">
-        <v>167</v>
+        <v>16</v>
       </c>
       <c r="AE43" s="2" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
       <c r="AI43" t="s">
-        <v>170</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add my name to spreadsheet
</commit_message>
<xml_diff>
--- a/reports/Protocol_test_Kendall.xlsx
+++ b/reports/Protocol_test_Kendall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bkendall/Documents/github-bitbucket/MPM-errors/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AE384825-AFFC-9849-9232-58E3C1BFA2A5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EB055648-5EB9-7146-8C8A-08C4D892BF7C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="460" windowWidth="32560" windowHeight="19940" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="228">
   <si>
     <t>CompadrinoName</t>
   </si>
@@ -708,6 +708,9 @@
   </si>
   <si>
     <t>Between the one-day timestep and the very high adult survival, errors due to improper formulation of the post-breeding census will be minor</t>
+  </si>
+  <si>
+    <t>Bruce Kendall</t>
   </si>
 </sst>
 </file>
@@ -1078,10 +1081,10 @@
   <dimension ref="A1:AK43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="11" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="11" topLeftCell="J19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="AK16" sqref="AK16"/>
+      <selection pane="bottomRight" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1386,6 +1389,9 @@
       </c>
     </row>
     <row r="12" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>227</v>
+      </c>
       <c r="C12" t="s">
         <v>154</v>
       </c>
@@ -1439,6 +1445,9 @@
       </c>
     </row>
     <row r="13" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>227</v>
+      </c>
       <c r="C13" t="s">
         <v>157</v>
       </c>
@@ -1489,6 +1498,9 @@
       </c>
     </row>
     <row r="14" spans="1:37" ht="208" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>227</v>
+      </c>
       <c r="C14" t="s">
         <v>70</v>
       </c>
@@ -1548,6 +1560,9 @@
       </c>
     </row>
     <row r="15" spans="1:37" ht="128" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>227</v>
+      </c>
       <c r="C15" t="s">
         <v>73</v>
       </c>
@@ -1610,6 +1625,9 @@
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>227</v>
+      </c>
       <c r="C16" t="s">
         <v>76</v>
       </c>
@@ -1644,7 +1662,10 @@
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>227</v>
+      </c>
       <c r="C17" t="s">
         <v>79</v>
       </c>
@@ -1682,7 +1703,10 @@
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>227</v>
+      </c>
       <c r="C18" t="s">
         <v>83</v>
       </c>
@@ -1717,7 +1741,10 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>227</v>
+      </c>
       <c r="C19" t="s">
         <v>86</v>
       </c>
@@ -1752,7 +1779,10 @@
         <v>191</v>
       </c>
     </row>
-    <row r="20" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>227</v>
+      </c>
       <c r="C20" t="s">
         <v>88</v>
       </c>
@@ -1793,7 +1823,10 @@
         <v>192</v>
       </c>
     </row>
-    <row r="21" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>227</v>
+      </c>
       <c r="C21" t="s">
         <v>91</v>
       </c>
@@ -1828,7 +1861,10 @@
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>227</v>
+      </c>
       <c r="C22" t="s">
         <v>94</v>
       </c>
@@ -1863,7 +1899,10 @@
         <v>193</v>
       </c>
     </row>
-    <row r="23" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>227</v>
+      </c>
       <c r="C23" t="s">
         <v>97</v>
       </c>
@@ -1898,7 +1937,10 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="3:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>227</v>
+      </c>
       <c r="C24" t="s">
         <v>100</v>
       </c>
@@ -1936,7 +1978,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>227</v>
+      </c>
       <c r="C25" t="s">
         <v>103</v>
       </c>
@@ -1971,7 +2016,10 @@
         <v>195</v>
       </c>
     </row>
-    <row r="26" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>227</v>
+      </c>
       <c r="C26" t="s">
         <v>105</v>
       </c>
@@ -2003,7 +2051,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>227</v>
+      </c>
       <c r="C27" t="s">
         <v>107</v>
       </c>
@@ -2035,7 +2086,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>227</v>
+      </c>
       <c r="C28" t="s">
         <v>158</v>
       </c>
@@ -2070,7 +2124,10 @@
         <v>196</v>
       </c>
     </row>
-    <row r="29" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>227</v>
+      </c>
       <c r="C29" t="s">
         <v>159</v>
       </c>
@@ -2105,7 +2162,10 @@
         <v>197</v>
       </c>
     </row>
-    <row r="30" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>227</v>
+      </c>
       <c r="C30" t="s">
         <v>113</v>
       </c>
@@ -2140,7 +2200,10 @@
         <v>198</v>
       </c>
     </row>
-    <row r="31" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>227</v>
+      </c>
       <c r="C31" t="s">
         <v>116</v>
       </c>
@@ -2162,7 +2225,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>227</v>
+      </c>
       <c r="C32" t="s">
         <v>116</v>
       </c>
@@ -2184,7 +2250,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="33" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>227</v>
+      </c>
       <c r="C33" t="s">
         <v>121</v>
       </c>
@@ -2219,7 +2288,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>227</v>
+      </c>
       <c r="C34" t="s">
         <v>124</v>
       </c>
@@ -2251,7 +2323,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>227</v>
+      </c>
       <c r="C35" t="s">
         <v>127</v>
       </c>
@@ -2267,7 +2342,10 @@
       <c r="AC35" s="2"/>
       <c r="AE35" s="2"/>
     </row>
-    <row r="36" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>227</v>
+      </c>
       <c r="C36" t="s">
         <v>130</v>
       </c>
@@ -2286,7 +2364,10 @@
         <v>201</v>
       </c>
     </row>
-    <row r="37" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>227</v>
+      </c>
       <c r="C37" t="s">
         <v>133</v>
       </c>
@@ -2318,7 +2399,10 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>227</v>
+      </c>
       <c r="C38" t="s">
         <v>136</v>
       </c>
@@ -2356,7 +2440,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>227</v>
+      </c>
       <c r="C39" t="s">
         <v>140</v>
       </c>
@@ -2388,7 +2475,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>227</v>
+      </c>
       <c r="C40" t="s">
         <v>143</v>
       </c>
@@ -2420,7 +2510,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>227</v>
+      </c>
       <c r="C41" t="s">
         <v>146</v>
       </c>
@@ -2452,7 +2545,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>227</v>
+      </c>
       <c r="C42" t="s">
         <v>148</v>
       </c>
@@ -2487,7 +2583,10 @@
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="3:37" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>227</v>
+      </c>
       <c r="C43" t="s">
         <v>152</v>
       </c>

</xml_diff>

<commit_message>
First attempt by the compadrinos on the protocol; BK's updates to his answers
</commit_message>
<xml_diff>
--- a/reports/Protocol_test_Kendall.xlsx
+++ b/reports/Protocol_test_Kendall.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bkendall/Documents/github-bitbucket/MPM-errors/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EB055648-5EB9-7146-8C8A-08C4D892BF7C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FEEFC0E9-1010-AA4B-A5A8-911E7DFFC884}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="460" windowWidth="32560" windowHeight="19940" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
+    <workbookView xWindow="8560" yWindow="7800" windowWidth="32560" windowHeight="19940" xr2:uid="{6865F7E1-48B8-E444-B55F-FEB41A06649B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="230">
   <si>
     <t>CompadrinoName</t>
   </si>
@@ -673,9 +673,6 @@
     <t>Observation</t>
   </si>
   <si>
-    <t>Comadre values for F1,3 differ from paper ("medium" matrix is shown on p. 214); I do not see how Comadre values of F1,3 could have been derived from lower level parameters (Table 1) for any of the models.</t>
-  </si>
-  <si>
     <t>Youngest class is called "fawn"; Fertility transitions include parent survival</t>
   </si>
   <si>
@@ -711,6 +708,15 @@
   </si>
   <si>
     <t>Bruce Kendall</t>
+  </si>
+  <si>
+    <t>Comadre values for F1,3 differ from paper ("medium" matrix is shown on p. 214); I do not see how Comadre values of F1,3 could have been derived from lower level parameters (Table 1) for this model.</t>
+  </si>
+  <si>
+    <t>2-year-olds are just transitioning into the adult stage, so first reproduction is as adult.</t>
+  </si>
+  <si>
+    <t>Post-breeding census means that "Yearling" reproduction is at age 2, as they mature into adults. This matches the interpretation of the life history</t>
   </si>
 </sst>
 </file>
@@ -1081,10 +1087,10 @@
   <dimension ref="A1:AK43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="11" topLeftCell="J19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="11" topLeftCell="Y12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="C41" sqref="C41"/>
+      <selection pane="bottomRight" activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1390,7 +1396,7 @@
     </row>
     <row r="12" spans="1:37" ht="144" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C12" t="s">
         <v>154</v>
@@ -1446,7 +1452,7 @@
     </row>
     <row r="13" spans="1:37" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C13" t="s">
         <v>157</v>
@@ -1497,9 +1503,9 @@
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="208" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" ht="144" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C14" t="s">
         <v>70</v>
@@ -1517,7 +1523,7 @@
         <v>8</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="O14" t="s">
         <v>214</v>
@@ -1529,23 +1535,32 @@
         <v>11</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="U14" t="s">
         <v>18</v>
       </c>
       <c r="V14" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="W14">
         <v>2</v>
       </c>
       <c r="X14" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>212</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>228</v>
       </c>
       <c r="AA14" t="s">
         <v>8</v>
       </c>
+      <c r="AB14" s="4" t="s">
+        <v>229</v>
+      </c>
       <c r="AC14" s="2" t="s">
         <v>16</v>
       </c>
@@ -1561,7 +1576,7 @@
     </row>
     <row r="15" spans="1:37" ht="128" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C15" t="s">
         <v>73</v>
@@ -1582,31 +1597,31 @@
         <v>11</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="U15" t="s">
         <v>16</v>
       </c>
       <c r="V15" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="W15">
         <v>365</v>
       </c>
       <c r="X15" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y15" t="s">
         <v>222</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>223</v>
       </c>
       <c r="AA15" t="s">
         <v>9</v>
       </c>
       <c r="AB15" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AC15" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AE15" s="2" t="s">
         <v>174</v>
@@ -1618,15 +1633,15 @@
         <v>27</v>
       </c>
       <c r="AJ15" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="AK15" t="s">
         <v>225</v>
-      </c>
-      <c r="AK15" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C16" t="s">
         <v>76</v>
@@ -1664,7 +1679,7 @@
     </row>
     <row r="17" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C17" t="s">
         <v>79</v>
@@ -1705,7 +1720,7 @@
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C18" t="s">
         <v>83</v>
@@ -1743,7 +1758,7 @@
     </row>
     <row r="19" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C19" t="s">
         <v>86</v>
@@ -1781,7 +1796,7 @@
     </row>
     <row r="20" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C20" t="s">
         <v>88</v>
@@ -1825,7 +1840,7 @@
     </row>
     <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C21" t="s">
         <v>91</v>
@@ -1863,7 +1878,7 @@
     </row>
     <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C22" t="s">
         <v>94</v>
@@ -1901,7 +1916,7 @@
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C23" t="s">
         <v>97</v>
@@ -1939,7 +1954,7 @@
     </row>
     <row r="24" spans="1:37" ht="80" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C24" t="s">
         <v>100</v>
@@ -1980,7 +1995,7 @@
     </row>
     <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C25" t="s">
         <v>103</v>
@@ -2018,7 +2033,7 @@
     </row>
     <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C26" t="s">
         <v>105</v>
@@ -2053,7 +2068,7 @@
     </row>
     <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C27" t="s">
         <v>107</v>
@@ -2088,7 +2103,7 @@
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C28" t="s">
         <v>158</v>
@@ -2126,7 +2141,7 @@
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C29" t="s">
         <v>159</v>
@@ -2164,7 +2179,7 @@
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C30" t="s">
         <v>113</v>
@@ -2202,7 +2217,7 @@
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C31" t="s">
         <v>116</v>
@@ -2227,7 +2242,7 @@
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C32" t="s">
         <v>116</v>
@@ -2252,7 +2267,7 @@
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C33" t="s">
         <v>121</v>
@@ -2290,7 +2305,7 @@
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C34" t="s">
         <v>124</v>
@@ -2325,7 +2340,7 @@
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C35" t="s">
         <v>127</v>
@@ -2344,7 +2359,7 @@
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C36" t="s">
         <v>130</v>
@@ -2366,7 +2381,7 @@
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C37" t="s">
         <v>133</v>
@@ -2401,7 +2416,7 @@
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C38" t="s">
         <v>136</v>
@@ -2442,7 +2457,7 @@
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C39" t="s">
         <v>140</v>
@@ -2477,7 +2492,7 @@
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C40" t="s">
         <v>143</v>
@@ -2512,7 +2527,7 @@
     </row>
     <row r="41" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C41" t="s">
         <v>146</v>
@@ -2547,7 +2562,7 @@
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C42" t="s">
         <v>148</v>
@@ -2585,7 +2600,7 @@
     </row>
     <row r="43" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C43" t="s">
         <v>152</v>

</xml_diff>